<commit_message>
added trimming to bulk dyn groups and all exit functions should now return
</commit_message>
<xml_diff>
--- a/Groups/DynamicGroupDbExcel.xlsx
+++ b/Groups/DynamicGroupDbExcel.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KielDavignonLab\Documents\EntraController\Groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6DA3FD-F030-4BC3-A6EF-82DD14D2C19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB134F34-9D69-4BF2-8FFB-9DF369B4A1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="14400" xr2:uid="{0601A4ED-7052-47BD-AF77-4EEBA4A2B09B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38610" windowHeight="14385" xr2:uid="{0601A4ED-7052-47BD-AF77-4EEBA4A2B09B}"/>
   </bookViews>
   <sheets>
     <sheet name="DynamicGroupDb" sheetId="2" r:id="rId1"/>
     <sheet name="ValidRules" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ValidRules!$A$1:$D$47</definedName>
     <definedName name="AndOrList">ValidRules!$C$2:$C$3</definedName>
     <definedName name="FilterOperators">ValidRules!$B$2:$B$14</definedName>
     <definedName name="FilterOperatorsList">ValidRules!$B$2:$B$14</definedName>
     <definedName name="MailEnabledList">ValidRules!$D$2:$D$3</definedName>
-    <definedName name="ValidPropertiesList">ValidRules!$A$2:$A$32</definedName>
+    <definedName name="ValidPropertiesList">ValidRules!$A$2:$A$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="175">
   <si>
     <t>GroupQuery</t>
   </si>
@@ -515,13 +516,64 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>extensionAttribute1</t>
+  </si>
+  <si>
+    <t>extensionAttribute2</t>
+  </si>
+  <si>
+    <t>extensionAttribute3</t>
+  </si>
+  <si>
+    <t>extensionAttribute4</t>
+  </si>
+  <si>
+    <t>extensionAttribute5</t>
+  </si>
+  <si>
+    <t>extensionAttribute6</t>
+  </si>
+  <si>
+    <t>extensionAttribute7</t>
+  </si>
+  <si>
+    <t>extensionAttribute8</t>
+  </si>
+  <si>
+    <t>extensionAttribute9</t>
+  </si>
+  <si>
+    <t>extensionAttribute10</t>
+  </si>
+  <si>
+    <t>extensionAttribute11</t>
+  </si>
+  <si>
+    <t>extensionAttribute12</t>
+  </si>
+  <si>
+    <t>extensionAttribute13</t>
+  </si>
+  <si>
+    <t>extensionAttribute14</t>
+  </si>
+  <si>
+    <t>extensionAttribute15</t>
+  </si>
+  <si>
+    <t>exttest</t>
+  </si>
+  <si>
+    <t>ExtTest2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,14 +714,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -980,7 +1024,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1023,16 +1067,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1066,7 +1108,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1407,15 +1448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239CD6A1-637D-4F3D-8D86-F5D570E0B934}">
-  <dimension ref="A1:DC12"/>
+  <dimension ref="A1:DC2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78.140625" customWidth="1"/>
+    <col min="1" max="1" width="105.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
@@ -1978,10 +2019,10 @@
     "(user." &amp; DA2 &amp; " -" &amp; DB2 &amp; " " &amp;
     IF(OR(DC2=TRUE, DC2=FALSE), DC2, CHAR(34) &amp; DC2 &amp; CHAR(34)) &amp; ")"
 )</f>
-        <v>(user.jobTitle -eq "Title")</v>
+        <v>(user.jobTitle -eq "Title") and (user.extensionAttribute1 -eq "exttest") or (user.extensionAttribute2 -contains "5")</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
         <v>156</v>
@@ -1998,27 +2039,47 @@
       <c r="G2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="12" spans="1:107" x14ac:dyDescent="0.25">
-      <c r="G12" s="4"/>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>159</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CW2:CW1048576 U2:U1048576 I2:I1048576 Q2:Q1048576 DA2:DA1048576 M2:M1048576 Y2:Y1048576 AC2:AC1048576 AG2:AG1048576 AK2:AK1048576 AO2:AO1048576 AS2:AS1048576 AW2:AW1048576 BA2:BA1048576 BE2:BE1048576 BI2:BI1048576 BM2:BM1048576 BQ2:BQ1048576 BU2:BU1048576 BY2:BY1048576 CC2:CC1048576 CG2:CG1048576 CK2:CK1048576 CO2:CO1048576 CS2:CS1048576 E2:E1048576" xr:uid="{F5F84789-440F-4E5C-AB73-B1A303AC4164}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576 CS2:CS1048576 CO2:CO1048576 CK2:CK1048576 CG2:CG1048576 CC2:CC1048576 BY2:BY1048576 BU2:BU1048576 BQ2:BQ1048576 BM2:BM1048576 BI2:BI1048576 BE2:BE1048576 BA2:BA1048576 AW2:AW1048576 AS2:AS1048576 AO2:AO1048576 AK2:AK1048576 AG2:AG1048576 AC2:AC1048576 Y2:Y1048576 M2:M1048576 DA2:DA1048576 Q2:Q1048576 I2:I1048576 U2:U1048576 CW2:CW1048576" xr:uid="{F5F84789-440F-4E5C-AB73-B1A303AC4164}">
       <formula1>ValidPropertiesList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CT2:CT1048576 V2:V1048576 CP2:CP1048576 R2:R1048576 CX2:CX1048576 DB2:DB1048576 N2:N1048576 Z2:Z1048576 AD2:AD1048576 AH2:AH1048576 AL2:AL1048576 AP2:AP1048576 AT2:AT1048576 AX2:AX1048576 BB2:BB1048576 BF2:BF1048576 BJ2:BJ1048576 BN2:BN1048576 BR2:BR1048576 BV2:BV1048576 BZ2:BZ1048576 CD2:CD1048576 CH2:CH1048576 CL2:CL1048576" xr:uid="{6F988CC4-F14B-4F69-8374-197884007D89}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2:CL1048576 CH2:CH1048576 CD2:CD1048576 BZ2:BZ1048576 BV2:BV1048576 BR2:BR1048576 BN2:BN1048576 BJ2:BJ1048576 BF2:BF1048576 BB2:BB1048576 AX2:AX1048576 AT2:AT1048576 AP2:AP1048576 AL2:AL1048576 AH2:AH1048576 AD2:AD1048576 Z2:Z1048576 N2:N1048576 DB2:DB1048576 CX2:CX1048576 R2:R1048576 CP2:CP1048576 V2:V1048576 CT2:CT1048576" xr:uid="{6F988CC4-F14B-4F69-8374-197884007D89}">
       <formula1>FilterOperatorsList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576 P2:P1048576 L2:L1048576 H2:H1048576 CZ2:CZ1048576 X2:X1048576 AB2:AB1048576 AF2:AF1048576 AJ2:AJ1048576 AN2:AN1048576 AR2:AR1048576 AV2:AV1048576 AZ2:AZ1048576 BD2:BD1048576 BH2:BH1048576 BL2:BL1048576 BP2:BP1048576 BT2:BT1048576 BX2:BX1048576 CB2:CB1048576 CF2:CF1048576 CJ2:CJ1048576 CN2:CN1048576 CR2:CR1048576 CV2:CV1048576" xr:uid="{347D2EE9-842B-45A4-A653-01EE1CAFE470}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CV2:CV1048576 CR2:CR1048576 CN2:CN1048576 CJ2:CJ1048576 CF2:CF1048576 CB2:CB1048576 BX2:BX1048576 BT2:BT1048576 BP2:BP1048576 BL2:BL1048576 BH2:BH1048576 BD2:BD1048576 AZ2:AZ1048576 AV2:AV1048576 AR2:AR1048576 AN2:AN1048576 AJ2:AJ1048576 AF2:AF1048576 AB2:AB1048576 X2:X1048576 CZ2:CZ1048576 H2:H1048576 L2:L1048576 P2:P1048576 T2:T1048576" xr:uid="{347D2EE9-842B-45A4-A653-01EE1CAFE470}">
       <formula1>AndOrList</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{2E83A840-977B-4ED3-B2CC-4092E3129D1D}">
       <formula1>MailEnabledList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 J2:J1048576" xr:uid="{3D4CBA15-A682-4B7D-AAF5-ADB3FA265A2A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576 F2:F1048576" xr:uid="{3D4CBA15-A682-4B7D-AAF5-ADB3FA265A2A}">
       <formula1>FilterOperators</formula1>
     </dataValidation>
   </dataValidations>
@@ -2029,10 +2090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5F8A4F-88C4-402B-90DC-6F88D50B5080}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,7 +2323,83 @@
         <v>35</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B14" xr:uid="{4513C465-84B3-4EFB-AD97-A48077BCA326}">
       <formula1>FilterOperators</formula1>

</xml_diff>